<commit_message>
Skips already archived; flags in source when archived
</commit_message>
<xml_diff>
--- a/master_fantasy_book_list.xlsx
+++ b/master_fantasy_book_list.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\p\gls01_workspace\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09B38B57-0AD2-4001-982F-A8720A07AC5A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89BAC79E-190A-48EC-8508-5B8AA3AEFA6F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="77">
   <si>
     <t>format</t>
   </si>
@@ -173,13 +173,94 @@
   </si>
   <si>
     <t>note</t>
+  </si>
+  <si>
+    <t>Scroll</t>
+  </si>
+  <si>
+    <t>Parchment</t>
+  </si>
+  <si>
+    <t>Elvish</t>
+  </si>
+  <si>
+    <t>Healing</t>
+  </si>
+  <si>
+    <t>Summarizing Healing: a Clandestine Expedition</t>
+  </si>
+  <si>
+    <t>Her Holiness Iuno Ocratia</t>
+  </si>
+  <si>
+    <t>Tofn telyg thynd</t>
+  </si>
+  <si>
+    <t>Iuno Ocratia</t>
+  </si>
+  <si>
+    <t>_names_roman_surnames</t>
+  </si>
+  <si>
+    <t>Her Holiness</t>
+  </si>
+  <si>
+    <t>Female</t>
+  </si>
+  <si>
+    <t>{verbing} {topic}: a {adjective_1} {noun_1}</t>
+  </si>
+  <si>
+    <t>Standard</t>
+  </si>
+  <si>
+    <t>e2eb8a74-3a9d-4b3c-8d45-bbf9ff65699d</t>
+  </si>
+  <si>
+    <t>has_been_archived</t>
+  </si>
+  <si>
+    <t>Codex</t>
+  </si>
+  <si>
+    <t>Vellum</t>
+  </si>
+  <si>
+    <t>Common</t>
+  </si>
+  <si>
+    <t>Contemplation</t>
+  </si>
+  <si>
+    <t>The Sins of Ásvaldr Eriksen, on the Subject of Contemplation</t>
+  </si>
+  <si>
+    <t>Duchess Nahla Soueid the Theologian</t>
+  </si>
+  <si>
+    <t>the Theologian</t>
+  </si>
+  <si>
+    <t>Nahla Soueid</t>
+  </si>
+  <si>
+    <t>_names_arabic_surnames</t>
+  </si>
+  <si>
+    <t>Duchess</t>
+  </si>
+  <si>
+    <t>{the_1} {negative_1} of {person_1}, on the Subject of {topic}</t>
+  </si>
+  <si>
+    <t>7a7158b0-eeaa-4c61-bcba-3f3cfd6a65f3</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -198,6 +279,14 @@
       <b/>
       <sz val="9"/>
       <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <name val="Tengwar Annatar"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <name val="Segoe UI Historic"/>
     </font>
   </fonts>
   <fills count="2">
@@ -220,7 +309,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -236,6 +325,8 @@
     <xf numFmtId="10" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -538,10 +629,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AX1"/>
+  <dimension ref="A1:AX3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -580,8 +671,8 @@
     <col min="41" max="48" width="9.140625" style="1" customWidth="1"/>
     <col min="49" max="49" width="37.140625" style="1" customWidth="1"/>
     <col min="50" max="50" width="18.140625" style="1" customWidth="1"/>
-    <col min="51" max="65" width="9.140625" style="1" customWidth="1"/>
-    <col min="66" max="16384" width="9.140625" style="1"/>
+    <col min="51" max="68" width="9.140625" style="1" customWidth="1"/>
+    <col min="69" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:50" x14ac:dyDescent="0.25">
@@ -734,6 +825,265 @@
       </c>
       <c r="AX1" s="4" t="s">
         <v>49</v>
+      </c>
+    </row>
+    <row r="2" spans="1:50" ht="17.25" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>50</v>
+      </c>
+      <c r="B2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C2">
+        <v>3</v>
+      </c>
+      <c r="D2">
+        <v>667</v>
+      </c>
+      <c r="E2">
+        <v>47</v>
+      </c>
+      <c r="F2" t="s">
+        <v>52</v>
+      </c>
+      <c r="H2" t="s">
+        <v>53</v>
+      </c>
+      <c r="I2" t="s">
+        <v>53</v>
+      </c>
+      <c r="J2">
+        <v>2</v>
+      </c>
+      <c r="K2">
+        <v>0</v>
+      </c>
+      <c r="L2">
+        <v>3</v>
+      </c>
+      <c r="M2">
+        <v>0</v>
+      </c>
+      <c r="N2">
+        <v>1</v>
+      </c>
+      <c r="O2">
+        <v>658</v>
+      </c>
+      <c r="P2" t="s">
+        <v>54</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>55</v>
+      </c>
+      <c r="S2" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="T2">
+        <v>4</v>
+      </c>
+      <c r="U2">
+        <v>4</v>
+      </c>
+      <c r="V2">
+        <v>1290</v>
+      </c>
+      <c r="W2">
+        <v>33</v>
+      </c>
+      <c r="X2">
+        <v>32</v>
+      </c>
+      <c r="Y2">
+        <v>0.25</v>
+      </c>
+      <c r="AB2" t="s">
+        <v>57</v>
+      </c>
+      <c r="AC2" t="s">
+        <v>58</v>
+      </c>
+      <c r="AD2" t="s">
+        <v>59</v>
+      </c>
+      <c r="AE2" t="s">
+        <v>60</v>
+      </c>
+      <c r="AJ2">
+        <v>0.06</v>
+      </c>
+      <c r="AK2" t="s">
+        <v>61</v>
+      </c>
+      <c r="AL2" t="s">
+        <v>53</v>
+      </c>
+      <c r="AM2">
+        <v>0.36</v>
+      </c>
+      <c r="AN2">
+        <v>241</v>
+      </c>
+      <c r="AO2">
+        <v>2.5</v>
+      </c>
+      <c r="AP2">
+        <v>417</v>
+      </c>
+      <c r="AQ2">
+        <v>0</v>
+      </c>
+      <c r="AR2">
+        <v>0</v>
+      </c>
+      <c r="AS2">
+        <v>0</v>
+      </c>
+      <c r="AT2">
+        <v>0</v>
+      </c>
+      <c r="AU2" t="b">
+        <v>0</v>
+      </c>
+      <c r="AV2" t="s">
+        <v>62</v>
+      </c>
+      <c r="AW2" t="s">
+        <v>63</v>
+      </c>
+      <c r="AX2" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="3" spans="1:50" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>65</v>
+      </c>
+      <c r="B3" t="s">
+        <v>66</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3">
+        <v>500</v>
+      </c>
+      <c r="E3">
+        <v>32</v>
+      </c>
+      <c r="F3" t="s">
+        <v>67</v>
+      </c>
+      <c r="H3" t="s">
+        <v>68</v>
+      </c>
+      <c r="I3" t="s">
+        <v>68</v>
+      </c>
+      <c r="J3">
+        <v>2</v>
+      </c>
+      <c r="K3">
+        <v>0</v>
+      </c>
+      <c r="L3">
+        <v>4</v>
+      </c>
+      <c r="M3">
+        <v>0</v>
+      </c>
+      <c r="N3">
+        <v>1</v>
+      </c>
+      <c r="O3">
+        <v>235</v>
+      </c>
+      <c r="P3" t="s">
+        <v>69</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>70</v>
+      </c>
+      <c r="S3" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="T3">
+        <v>3</v>
+      </c>
+      <c r="U3">
+        <v>3</v>
+      </c>
+      <c r="V3">
+        <v>32</v>
+      </c>
+      <c r="W3">
+        <v>414</v>
+      </c>
+      <c r="X3">
+        <v>413</v>
+      </c>
+      <c r="Y3">
+        <v>0.02</v>
+      </c>
+      <c r="AA3" t="s">
+        <v>71</v>
+      </c>
+      <c r="AB3" t="s">
+        <v>72</v>
+      </c>
+      <c r="AC3" t="s">
+        <v>73</v>
+      </c>
+      <c r="AD3" t="s">
+        <v>74</v>
+      </c>
+      <c r="AE3" t="s">
+        <v>60</v>
+      </c>
+      <c r="AJ3">
+        <v>0.06</v>
+      </c>
+      <c r="AK3" t="s">
+        <v>75</v>
+      </c>
+      <c r="AL3" t="s">
+        <v>68</v>
+      </c>
+      <c r="AM3">
+        <v>0.39</v>
+      </c>
+      <c r="AN3">
+        <v>195</v>
+      </c>
+      <c r="AO3">
+        <v>4</v>
+      </c>
+      <c r="AP3">
+        <v>40</v>
+      </c>
+      <c r="AQ3">
+        <v>0</v>
+      </c>
+      <c r="AR3">
+        <v>0</v>
+      </c>
+      <c r="AS3">
+        <v>0</v>
+      </c>
+      <c r="AT3">
+        <v>0</v>
+      </c>
+      <c r="AU3" t="b">
+        <v>0</v>
+      </c>
+      <c r="AV3" t="s">
+        <v>62</v>
+      </c>
+      <c r="AW3" t="s">
+        <v>76</v>
+      </c>
+      <c r="AX3" t="s">
+        <v>64</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
loops through master list properly, subtracting, and repeating if picks book with zero left to place
</commit_message>
<xml_diff>
--- a/master_fantasy_book_list.xlsx
+++ b/master_fantasy_book_list.xlsx
@@ -445,7 +445,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AX2"/>
+  <dimension ref="A1:AX3"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="T1" workbookViewId="0">
       <selection activeCell="X4" sqref="X4"/>
@@ -487,8 +487,8 @@
     <col width="9.140625" customWidth="1" style="1" min="41" max="48"/>
     <col width="37.140625" customWidth="1" style="1" min="49" max="49"/>
     <col width="18.140625" customWidth="1" style="1" min="50" max="50"/>
-    <col width="9.140625" customWidth="1" style="1" min="51" max="69"/>
-    <col width="9.140625" customWidth="1" style="1" min="70" max="16384"/>
+    <col width="9.140625" customWidth="1" style="1" min="51" max="70"/>
+    <col width="9.140625" customWidth="1" style="1" min="71" max="16384"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -824,7 +824,7 @@
         <v>10</v>
       </c>
       <c r="X2" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="Y2" t="n">
         <v>0.02</v>
@@ -900,6 +900,168 @@
         </is>
       </c>
       <c r="AX2" t="inlineStr">
+        <is>
+          <t>has_been_archived</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Codex</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Parchment</t>
+        </is>
+      </c>
+      <c r="C3" t="n">
+        <v>1</v>
+      </c>
+      <c r="D3" t="n">
+        <v>115</v>
+      </c>
+      <c r="E3" t="n">
+        <v>8</v>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>Regional</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>Craft (fletching)</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>Craft (fletching)</t>
+        </is>
+      </c>
+      <c r="J3" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="K3" t="n">
+        <v>0</v>
+      </c>
+      <c r="L3" t="n">
+        <v>2</v>
+      </c>
+      <c r="M3" t="n">
+        <v>0</v>
+      </c>
+      <c r="N3" t="n">
+        <v>0.23</v>
+      </c>
+      <c r="O3" t="n">
+        <v>46</v>
+      </c>
+      <c r="P3" t="inlineStr">
+        <is>
+          <t>The Peccability of Þórvaldr Olsdotter, on the Subject of Crafting of Arrows</t>
+        </is>
+      </c>
+      <c r="Q3" t="inlineStr">
+        <is>
+          <t>The Venerable Torhtsige Magnusson</t>
+        </is>
+      </c>
+      <c r="S3" s="7" t="inlineStr">
+        <is>
+          <t>Ἀπεναντίον περιφέρεια] ἐπίπεδος ὑπὸ ὀρθαῖς ἐὰν διάμετρος ἰσοσκελῶν δοθείσης ὅλον ἑκατέρᾳ] τρίπλευρα πάσας ἐν ιζ΄ τῆς τινος εἶναι</t>
+        </is>
+      </c>
+      <c r="T3" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="U3" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="V3" t="n">
+        <v>28</v>
+      </c>
+      <c r="W3" t="n">
+        <v>10</v>
+      </c>
+      <c r="X3" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y3" t="n">
+        <v>0.02</v>
+      </c>
+      <c r="AB3" t="inlineStr">
+        <is>
+          <t>Torhtsige Magnusson</t>
+        </is>
+      </c>
+      <c r="AC3" t="inlineStr">
+        <is>
+          <t>_names_norse_surnames_male</t>
+        </is>
+      </c>
+      <c r="AD3" t="inlineStr">
+        <is>
+          <t>The Venerable</t>
+        </is>
+      </c>
+      <c r="AE3" t="inlineStr">
+        <is>
+          <t>Male</t>
+        </is>
+      </c>
+      <c r="AJ3" t="n">
+        <v>0.06</v>
+      </c>
+      <c r="AK3" t="inlineStr">
+        <is>
+          <t>{the_1} {negative_1} of {person_1}, on the Subject of {topic}</t>
+        </is>
+      </c>
+      <c r="AL3" t="inlineStr">
+        <is>
+          <t>Crafting of Arrows</t>
+        </is>
+      </c>
+      <c r="AM3" t="n">
+        <v>0.37</v>
+      </c>
+      <c r="AN3" t="n">
+        <v>185</v>
+      </c>
+      <c r="AO3" t="n">
+        <v>1.25</v>
+      </c>
+      <c r="AP3" t="n">
+        <v>13</v>
+      </c>
+      <c r="AQ3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AR3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AT3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AU3" t="b">
+        <v>0</v>
+      </c>
+      <c r="AV3" t="inlineStr">
+        <is>
+          <t>Standard</t>
+        </is>
+      </c>
+      <c r="AW3" t="inlineStr">
+        <is>
+          <t>3865d234-5784-44ae-8fcd-0189dffddb49</t>
+        </is>
+      </c>
+      <c r="AX3" t="inlineStr">
         <is>
           <t>has_been_archived</t>
         </is>

</xml_diff>

<commit_message>
Works selecting preexisting books in proper ratio
</commit_message>
<xml_diff>
--- a/master_fantasy_book_list.xlsx
+++ b/master_fantasy_book_list.xlsx
@@ -18,7 +18,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
@@ -53,6 +53,10 @@
       <family val="2"/>
       <sz val="9"/>
     </font>
+    <font>
+      <name val="Segoe UI Historic"/>
+      <sz val="9"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -74,7 +78,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
@@ -100,6 +104,7 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -465,13 +470,13 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AX188"/>
+  <dimension ref="A1:AX201"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A172" workbookViewId="0">
       <selection activeCell="B188" sqref="B188"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15.75" outlineLevelCol="0"/>
   <cols>
     <col width="9.140625" customWidth="1" style="1" min="1" max="1"/>
     <col width="16.5703125" customWidth="1" style="1" min="2" max="2"/>
@@ -1664,7 +1669,7 @@
         <v>47</v>
       </c>
       <c r="X7" s="12" t="n">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="Y7" t="n">
         <v>0.25</v>
@@ -1821,7 +1826,7 @@
         <v>125</v>
       </c>
       <c r="X8" s="12" t="n">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="Y8" t="n">
         <v>0.05</v>
@@ -3107,7 +3112,7 @@
         <v>34</v>
       </c>
       <c r="X16" s="12" t="n">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="Y16" t="n">
         <v>0.25</v>
@@ -3264,7 +3269,7 @@
         <v>97</v>
       </c>
       <c r="X17" s="12" t="n">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="Y17" t="n">
         <v>0.1</v>
@@ -3892,7 +3897,7 @@
         <v>1451</v>
       </c>
       <c r="X21" s="12" t="n">
-        <v>1450</v>
+        <v>1446</v>
       </c>
       <c r="Y21" t="n">
         <v>0</v>
@@ -5325,7 +5330,7 @@
         <v>46</v>
       </c>
       <c r="X30" s="12" t="n">
-        <v>37</v>
+        <v>25</v>
       </c>
       <c r="Y30" t="n">
         <v>0.25</v>
@@ -5482,7 +5487,7 @@
         <v>571</v>
       </c>
       <c r="X31" s="12" t="n">
-        <v>568</v>
+        <v>560</v>
       </c>
       <c r="Y31" t="n">
         <v>0.01</v>
@@ -5639,7 +5644,7 @@
         <v>459</v>
       </c>
       <c r="X32" s="12" t="n">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="Y32" t="n">
         <v>0.02</v>
@@ -6115,7 +6120,7 @@
         <v>15</v>
       </c>
       <c r="X35" s="12" t="n">
-        <v>13</v>
+        <v>0</v>
       </c>
       <c r="Y35" t="n">
         <v>0.33</v>
@@ -6282,7 +6287,7 @@
         <v>749</v>
       </c>
       <c r="X36" s="12" t="n">
-        <v>726</v>
+        <v>722</v>
       </c>
       <c r="Y36" t="n">
         <v>0.01</v>
@@ -6444,7 +6449,7 @@
         <v>162</v>
       </c>
       <c r="X37" s="12" t="n">
-        <v>159</v>
+        <v>128</v>
       </c>
       <c r="Y37" t="n">
         <v>0.05</v>
@@ -6611,7 +6616,7 @@
         <v>1608</v>
       </c>
       <c r="X38" s="12" t="n">
-        <v>1605</v>
+        <v>1603</v>
       </c>
       <c r="Y38" t="n">
         <v>0</v>
@@ -7563,7 +7568,7 @@
         <v>15</v>
       </c>
       <c r="X44" s="12" t="n">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="Y44" t="n">
         <v>0.33</v>
@@ -7877,7 +7882,7 @@
         <v>3</v>
       </c>
       <c r="X46" s="12" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="Y46" t="n">
         <v>0.5</v>
@@ -8525,7 +8530,7 @@
         <v>27</v>
       </c>
       <c r="X50" s="12" t="n">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="Y50" t="n">
         <v>0.25</v>
@@ -11386,7 +11391,7 @@
         <v>42</v>
       </c>
       <c r="X68" s="12" t="n">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="Y68" t="n">
         <v>0.25</v>
@@ -11715,7 +11720,7 @@
         <v>18</v>
       </c>
       <c r="X70" s="12" t="n">
-        <v>17</v>
+        <v>1</v>
       </c>
       <c r="Y70" t="n">
         <v>0.33</v>
@@ -11897,7 +11902,7 @@
         <v>1031</v>
       </c>
       <c r="X71" s="12" t="n">
-        <v>1030</v>
+        <v>1029</v>
       </c>
       <c r="Y71" t="n">
         <v>0</v>
@@ -12059,7 +12064,7 @@
         <v>4</v>
       </c>
       <c r="X72" s="12" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="Y72" t="n">
         <v>0.5</v>
@@ -12712,7 +12717,7 @@
         <v>21</v>
       </c>
       <c r="X76" s="12" t="n">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="Y76" t="n">
         <v>0.33</v>
@@ -12874,7 +12879,7 @@
         <v>138</v>
       </c>
       <c r="X77" s="12" t="n">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="Y77" t="n">
         <v>0.05</v>
@@ -13193,7 +13198,7 @@
         <v>24</v>
       </c>
       <c r="X79" s="12" t="n">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="Y79" t="n">
         <v>0.33</v>
@@ -13826,7 +13831,7 @@
         <v>71</v>
       </c>
       <c r="X83" s="12" t="n">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="Y83" t="n">
         <v>0.1</v>
@@ -13988,7 +13993,7 @@
         <v>316</v>
       </c>
       <c r="X84" s="12" t="n">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="Y84" t="n">
         <v>0.02</v>
@@ -14616,7 +14621,7 @@
         <v>2</v>
       </c>
       <c r="X88" s="12" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Y88" t="n">
         <v>0.5</v>
@@ -14935,7 +14940,7 @@
         <v>3</v>
       </c>
       <c r="X90" s="12" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Y90" t="n">
         <v>0.5</v>
@@ -15097,7 +15102,7 @@
         <v>936</v>
       </c>
       <c r="X91" s="12" t="n">
-        <v>935</v>
+        <v>934</v>
       </c>
       <c r="Y91" t="n">
         <v>0.01</v>
@@ -15411,7 +15416,7 @@
         <v>6</v>
       </c>
       <c r="X93" s="12" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="Y93" t="n">
         <v>0.33</v>
@@ -15568,7 +15573,7 @@
         <v>38</v>
       </c>
       <c r="X94" s="12" t="n">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="Y94" t="n">
         <v>0.25</v>
@@ -15725,7 +15730,7 @@
         <v>115</v>
       </c>
       <c r="X95" s="12" t="n">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="Y95" t="n">
         <v>0.05</v>
@@ -16049,7 +16054,7 @@
         <v>43</v>
       </c>
       <c r="X97" s="12" t="n">
-        <v>42</v>
+        <v>30</v>
       </c>
       <c r="Y97" t="n">
         <v>0.25</v>
@@ -16530,7 +16535,7 @@
         <v>250</v>
       </c>
       <c r="X100" s="12" t="n">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="Y100" t="n">
         <v>0.05</v>
@@ -16849,7 +16854,7 @@
         <v>4</v>
       </c>
       <c r="X102" s="12" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="Y102" t="n">
         <v>0.5</v>
@@ -17659,7 +17664,7 @@
         <v>2</v>
       </c>
       <c r="X107" s="12" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Y107" t="n">
         <v>0.5</v>
@@ -18312,7 +18317,7 @@
         <v>31</v>
       </c>
       <c r="X111" s="12" t="n">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="Y111" t="n">
         <v>0.25</v>
@@ -19421,7 +19426,7 @@
         <v>4</v>
       </c>
       <c r="X118" s="12" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="Y118" t="n">
         <v>0.5</v>
@@ -19578,7 +19583,7 @@
         <v>413</v>
       </c>
       <c r="X119" s="12" t="n">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="Y119" t="n">
         <v>0.02</v>
@@ -20059,7 +20064,7 @@
         <v>826</v>
       </c>
       <c r="X122" s="12" t="n">
-        <v>824</v>
+        <v>821</v>
       </c>
       <c r="Y122" t="n">
         <v>0.01</v>
@@ -20216,7 +20221,7 @@
         <v>253</v>
       </c>
       <c r="X123" s="12" t="n">
-        <v>249</v>
+        <v>242</v>
       </c>
       <c r="Y123" t="n">
         <v>0.02</v>
@@ -20373,7 +20378,7 @@
         <v>146</v>
       </c>
       <c r="X124" s="12" t="n">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="Y124" t="n">
         <v>0.05</v>
@@ -20535,7 +20540,7 @@
         <v>264</v>
       </c>
       <c r="X125" s="12" t="n">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="Y125" t="n">
         <v>0.02</v>
@@ -21330,7 +21335,7 @@
         <v>2</v>
       </c>
       <c r="X130" s="12" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Y130" t="n">
         <v>0.5</v>
@@ -22155,7 +22160,7 @@
         <v>23</v>
       </c>
       <c r="X135" s="12" t="n">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="Y135" t="n">
         <v>0.33</v>
@@ -22474,7 +22479,7 @@
         <v>7</v>
       </c>
       <c r="X137" s="12" t="n">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="Y137" t="n">
         <v>0.33</v>
@@ -23598,7 +23603,7 @@
         <v>26</v>
       </c>
       <c r="X144" s="12" t="n">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="Y144" t="n">
         <v>0.25</v>
@@ -24069,7 +24074,7 @@
         <v>135</v>
       </c>
       <c r="X147" s="12" t="n">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="Y147" t="n">
         <v>0.05</v>
@@ -24226,7 +24231,7 @@
         <v>252</v>
       </c>
       <c r="X148" s="12" t="n">
-        <v>251</v>
+        <v>240</v>
       </c>
       <c r="Y148" t="n">
         <v>0.02</v>
@@ -25021,7 +25026,7 @@
         <v>5</v>
       </c>
       <c r="X153" s="12" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="Y153" t="n">
         <v>0.5</v>
@@ -25183,7 +25188,7 @@
         <v>232</v>
       </c>
       <c r="X154" s="12" t="n">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="Y154" t="n">
         <v>0.05</v>
@@ -26145,7 +26150,7 @@
         <v>7</v>
       </c>
       <c r="X160" s="12" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="Y160" t="n">
         <v>0.33</v>
@@ -26484,7 +26489,7 @@
         <v>8</v>
       </c>
       <c r="X162" s="12" t="n">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="Y162" t="n">
         <v>0.33</v>
@@ -26641,7 +26646,7 @@
         <v>953</v>
       </c>
       <c r="X163" s="12" t="n">
-        <v>952</v>
+        <v>951</v>
       </c>
       <c r="Y163" t="n">
         <v>0.01</v>
@@ -28306,7 +28311,7 @@
         <v>30</v>
       </c>
       <c r="X173" s="12" t="n">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="Y173" t="n">
         <v>0.25</v>
@@ -28463,7 +28468,7 @@
         <v>14</v>
       </c>
       <c r="X174" s="12" t="n">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="Y174" t="n">
         <v>0.33</v>
@@ -28635,7 +28640,7 @@
         <v>87</v>
       </c>
       <c r="X175" s="12" t="n">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="Y175" t="n">
         <v>0.1</v>
@@ -28807,7 +28812,7 @@
         <v>62</v>
       </c>
       <c r="X176" s="12" t="n">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="Y176" t="n">
         <v>0.1</v>
@@ -29126,7 +29131,7 @@
         <v>59</v>
       </c>
       <c r="X178" s="12" t="n">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="Y178" t="n">
         <v>0.1</v>
@@ -29283,7 +29288,7 @@
         <v>166</v>
       </c>
       <c r="X179" s="12" t="n">
-        <v>165</v>
+        <v>154</v>
       </c>
       <c r="Y179" t="n">
         <v>0.05</v>
@@ -29597,7 +29602,7 @@
         <v>12</v>
       </c>
       <c r="X181" s="12" t="n">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="Y181" t="n">
         <v>0.33</v>
@@ -29754,7 +29759,7 @@
         <v>44</v>
       </c>
       <c r="X182" s="12" t="n">
-        <v>43</v>
+        <v>14</v>
       </c>
       <c r="Y182" t="n">
         <v>0.25</v>
@@ -29916,7 +29921,7 @@
         <v>1972</v>
       </c>
       <c r="X183" s="12" t="n">
-        <v>1971</v>
+        <v>1949</v>
       </c>
       <c r="Y183" t="n">
         <v>0</v>
@@ -30230,7 +30235,7 @@
         <v>6</v>
       </c>
       <c r="X185" s="12" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="Y185" t="n">
         <v>0.33</v>
@@ -30782,6 +30787,2107 @@
         </is>
       </c>
       <c r="AX188" t="inlineStr">
+        <is>
+          <t>has_been_archived</t>
+        </is>
+      </c>
+    </row>
+    <row r="189">
+      <c r="A189" t="inlineStr">
+        <is>
+          <t>Codex</t>
+        </is>
+      </c>
+      <c r="B189" t="inlineStr">
+        <is>
+          <t>Vellum</t>
+        </is>
+      </c>
+      <c r="C189" t="n">
+        <v>2</v>
+      </c>
+      <c r="D189" t="n">
+        <v>510</v>
+      </c>
+      <c r="E189" t="n">
+        <v>33</v>
+      </c>
+      <c r="F189" t="inlineStr">
+        <is>
+          <t>Classical</t>
+        </is>
+      </c>
+      <c r="H189" t="inlineStr">
+        <is>
+          <t>Sniping</t>
+        </is>
+      </c>
+      <c r="I189" t="inlineStr">
+        <is>
+          <t>Sniping</t>
+        </is>
+      </c>
+      <c r="J189" t="n">
+        <v>1</v>
+      </c>
+      <c r="K189" t="n">
+        <v>0</v>
+      </c>
+      <c r="L189" t="n">
+        <v>1</v>
+      </c>
+      <c r="M189" t="n">
+        <v>0</v>
+      </c>
+      <c r="N189" t="n">
+        <v>0.51</v>
+      </c>
+      <c r="O189" t="n">
+        <v>327</v>
+      </c>
+      <c r="P189" t="inlineStr">
+        <is>
+          <t>Sniping, a Buried Circumference</t>
+        </is>
+      </c>
+      <c r="Q189" t="inlineStr">
+        <is>
+          <t>Pæga Whitley</t>
+        </is>
+      </c>
+      <c r="S189" s="13" t="inlineStr">
+        <is>
+          <t>Amicitia praedicavit liberi ordinum emittere arcem transitur</t>
+        </is>
+      </c>
+      <c r="T189" t="n">
+        <v>3</v>
+      </c>
+      <c r="U189" t="n">
+        <v>3</v>
+      </c>
+      <c r="V189" t="n">
+        <v>133</v>
+      </c>
+      <c r="W189" t="n">
+        <v>45</v>
+      </c>
+      <c r="X189" t="n">
+        <v>44</v>
+      </c>
+      <c r="Y189" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="AB189" t="inlineStr">
+        <is>
+          <t>Pæga Whitley</t>
+        </is>
+      </c>
+      <c r="AC189" t="inlineStr">
+        <is>
+          <t>_names_anglo_saxon_surnames</t>
+        </is>
+      </c>
+      <c r="AE189" t="inlineStr">
+        <is>
+          <t>Female</t>
+        </is>
+      </c>
+      <c r="AJ189" t="n">
+        <v>0.06</v>
+      </c>
+      <c r="AK189" t="inlineStr">
+        <is>
+          <t>{topic}, a {adjective_1} {noun_1}</t>
+        </is>
+      </c>
+      <c r="AL189" t="inlineStr">
+        <is>
+          <t>Sniping</t>
+        </is>
+      </c>
+      <c r="AM189" t="n">
+        <v>0.39</v>
+      </c>
+      <c r="AN189" t="n">
+        <v>390</v>
+      </c>
+      <c r="AO189" t="n">
+        <v>1</v>
+      </c>
+      <c r="AP189" t="n">
+        <v>250</v>
+      </c>
+      <c r="AQ189" t="n">
+        <v>0</v>
+      </c>
+      <c r="AR189" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS189" t="n">
+        <v>0</v>
+      </c>
+      <c r="AT189" t="n">
+        <v>0</v>
+      </c>
+      <c r="AU189" t="b">
+        <v>0</v>
+      </c>
+      <c r="AV189" t="inlineStr">
+        <is>
+          <t>Standard</t>
+        </is>
+      </c>
+      <c r="AW189" t="inlineStr">
+        <is>
+          <t>8fc0b27f-0809-4a72-9aab-8eef1b93048d</t>
+        </is>
+      </c>
+      <c r="AX189" t="inlineStr">
+        <is>
+          <t>has_been_archived</t>
+        </is>
+      </c>
+    </row>
+    <row r="190">
+      <c r="A190" t="inlineStr">
+        <is>
+          <t>Codex</t>
+        </is>
+      </c>
+      <c r="B190" t="inlineStr">
+        <is>
+          <t>Vellum</t>
+        </is>
+      </c>
+      <c r="C190" t="n">
+        <v>1</v>
+      </c>
+      <c r="D190" t="n">
+        <v>667</v>
+      </c>
+      <c r="E190" t="n">
+        <v>43</v>
+      </c>
+      <c r="F190" t="inlineStr">
+        <is>
+          <t>Common</t>
+        </is>
+      </c>
+      <c r="H190" t="inlineStr">
+        <is>
+          <t>Performance (playing instruments)</t>
+        </is>
+      </c>
+      <c r="I190" t="inlineStr">
+        <is>
+          <t>Performance (playing instruments)</t>
+        </is>
+      </c>
+      <c r="J190" t="n">
+        <v>2</v>
+      </c>
+      <c r="K190" t="n">
+        <v>0</v>
+      </c>
+      <c r="L190" t="n">
+        <v>3</v>
+      </c>
+      <c r="M190" t="n">
+        <v>0</v>
+      </c>
+      <c r="N190" t="n">
+        <v>1</v>
+      </c>
+      <c r="O190" t="n">
+        <v>1095</v>
+      </c>
+      <c r="P190" t="inlineStr">
+        <is>
+          <t>Correspondence Respecting The Seductive Lute of Eadwig Sweete</t>
+        </is>
+      </c>
+      <c r="Q190" t="inlineStr">
+        <is>
+          <t>Doctor Rodolphe Pedersen</t>
+        </is>
+      </c>
+      <c r="S190" s="13" t="inlineStr">
+        <is>
+          <t>Correspondence Respecting The Seductive Lute of Eadwig Sweete</t>
+        </is>
+      </c>
+      <c r="T190" t="n">
+        <v>4</v>
+      </c>
+      <c r="U190" t="n">
+        <v>4</v>
+      </c>
+      <c r="V190" t="n">
+        <v>43</v>
+      </c>
+      <c r="W190" t="n">
+        <v>4</v>
+      </c>
+      <c r="X190" t="n">
+        <v>3</v>
+      </c>
+      <c r="Y190" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="AB190" t="inlineStr">
+        <is>
+          <t>Rodolphe Pedersen</t>
+        </is>
+      </c>
+      <c r="AC190" t="inlineStr">
+        <is>
+          <t>_names_norse_surnames_male</t>
+        </is>
+      </c>
+      <c r="AD190" t="inlineStr">
+        <is>
+          <t>Doctor</t>
+        </is>
+      </c>
+      <c r="AE190" t="inlineStr">
+        <is>
+          <t>Male</t>
+        </is>
+      </c>
+      <c r="AJ190" t="n">
+        <v>0.06</v>
+      </c>
+      <c r="AK190" t="inlineStr">
+        <is>
+          <t>{communication} {conjunction_about} {topic} {conjunction_by} {person_1}</t>
+        </is>
+      </c>
+      <c r="AL190" t="inlineStr">
+        <is>
+          <t>The Seductive Lute</t>
+        </is>
+      </c>
+      <c r="AM190" t="n">
+        <v>0.39</v>
+      </c>
+      <c r="AN190" t="n">
+        <v>261</v>
+      </c>
+      <c r="AO190" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="AP190" t="n">
+        <v>834</v>
+      </c>
+      <c r="AQ190" t="n">
+        <v>0</v>
+      </c>
+      <c r="AR190" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS190" t="n">
+        <v>0</v>
+      </c>
+      <c r="AT190" t="n">
+        <v>0</v>
+      </c>
+      <c r="AU190" t="b">
+        <v>0</v>
+      </c>
+      <c r="AV190" t="inlineStr">
+        <is>
+          <t>Standard</t>
+        </is>
+      </c>
+      <c r="AW190" t="inlineStr">
+        <is>
+          <t>78be21f3-8256-4ebf-bf15-a9effdd08e8c</t>
+        </is>
+      </c>
+      <c r="AX190" t="inlineStr">
+        <is>
+          <t>has_been_archived</t>
+        </is>
+      </c>
+    </row>
+    <row r="191">
+      <c r="A191" t="inlineStr">
+        <is>
+          <t>Codex</t>
+        </is>
+      </c>
+      <c r="B191" t="inlineStr">
+        <is>
+          <t>Vellum</t>
+        </is>
+      </c>
+      <c r="C191" t="n">
+        <v>2</v>
+      </c>
+      <c r="D191" t="n">
+        <v>1000</v>
+      </c>
+      <c r="E191" t="n">
+        <v>63</v>
+      </c>
+      <c r="F191" t="inlineStr">
+        <is>
+          <t>Regional</t>
+        </is>
+      </c>
+      <c r="H191" t="inlineStr">
+        <is>
+          <t>Esoteric: Alchemy</t>
+        </is>
+      </c>
+      <c r="I191" t="inlineStr">
+        <is>
+          <t>Disguise</t>
+        </is>
+      </c>
+      <c r="J191" t="n">
+        <v>1</v>
+      </c>
+      <c r="K191" t="n">
+        <v>1</v>
+      </c>
+      <c r="L191" t="n">
+        <v>1</v>
+      </c>
+      <c r="M191" t="n">
+        <v>1</v>
+      </c>
+      <c r="N191" t="n">
+        <v>1</v>
+      </c>
+      <c r="O191" t="n">
+        <v>5720</v>
+      </c>
+      <c r="P191" t="inlineStr">
+        <is>
+          <t>The Regrettable Sloth of Azeena Kadir, on the Subject of Disguise</t>
+        </is>
+      </c>
+      <c r="Q191" t="inlineStr">
+        <is>
+          <t>Wilfrith Nutlee</t>
+        </is>
+      </c>
+      <c r="S191" s="13" t="inlineStr">
+        <is>
+          <t>Ὀρθογώνιον ἀμβλυγώνιον δοθέντι ἐστίν] ἀλλήλων λοιπῇ ς΄ περὶ ἥτις ἃ τῷ</t>
+        </is>
+      </c>
+      <c r="T191" t="n">
+        <v>6</v>
+      </c>
+      <c r="U191" t="n">
+        <v>6</v>
+      </c>
+      <c r="V191" t="n">
+        <v>16</v>
+      </c>
+      <c r="W191" t="n">
+        <v>11</v>
+      </c>
+      <c r="X191" t="n">
+        <v>10</v>
+      </c>
+      <c r="Y191" t="n">
+        <v>0.33</v>
+      </c>
+      <c r="AB191" t="inlineStr">
+        <is>
+          <t>Wilfrith Nutlee</t>
+        </is>
+      </c>
+      <c r="AC191" t="inlineStr">
+        <is>
+          <t>_names_anglo_saxon_surnames</t>
+        </is>
+      </c>
+      <c r="AE191" t="inlineStr">
+        <is>
+          <t>Female</t>
+        </is>
+      </c>
+      <c r="AJ191" t="n">
+        <v>0.06</v>
+      </c>
+      <c r="AK191" t="inlineStr">
+        <is>
+          <t>{the_1} {negative_1} of {person_1}, on the Subject of {topic}</t>
+        </is>
+      </c>
+      <c r="AL191" t="inlineStr">
+        <is>
+          <t>Disguise</t>
+        </is>
+      </c>
+      <c r="AM191" t="n">
+        <v>0.39</v>
+      </c>
+      <c r="AN191" t="n">
+        <v>390</v>
+      </c>
+      <c r="AO191" t="n">
+        <v>1</v>
+      </c>
+      <c r="AP191" t="n">
+        <v>330</v>
+      </c>
+      <c r="AQ191" t="n">
+        <v>1</v>
+      </c>
+      <c r="AR191" t="n">
+        <v>5000</v>
+      </c>
+      <c r="AS191" t="n">
+        <v>0</v>
+      </c>
+      <c r="AT191" t="n">
+        <v>0</v>
+      </c>
+      <c r="AU191" t="b">
+        <v>0</v>
+      </c>
+      <c r="AV191" t="inlineStr">
+        <is>
+          <t>Standard</t>
+        </is>
+      </c>
+      <c r="AW191" t="inlineStr">
+        <is>
+          <t>510746eb-ab56-4ce5-847f-afa987a3e739</t>
+        </is>
+      </c>
+      <c r="AX191" t="inlineStr">
+        <is>
+          <t>has_been_archived</t>
+        </is>
+      </c>
+    </row>
+    <row r="192">
+      <c r="A192" t="inlineStr">
+        <is>
+          <t>Codex</t>
+        </is>
+      </c>
+      <c r="B192" t="inlineStr">
+        <is>
+          <t>Vellum</t>
+        </is>
+      </c>
+      <c r="C192" t="n">
+        <v>2</v>
+      </c>
+      <c r="D192" t="n">
+        <v>1000</v>
+      </c>
+      <c r="E192" t="n">
+        <v>63</v>
+      </c>
+      <c r="F192" t="inlineStr">
+        <is>
+          <t>Regional</t>
+        </is>
+      </c>
+      <c r="H192" t="inlineStr">
+        <is>
+          <t>Dungeon Bashing</t>
+        </is>
+      </c>
+      <c r="I192" t="inlineStr">
+        <is>
+          <t>Dungeon Bashing</t>
+        </is>
+      </c>
+      <c r="J192" t="n">
+        <v>1</v>
+      </c>
+      <c r="K192" t="n">
+        <v>0</v>
+      </c>
+      <c r="L192" t="n">
+        <v>1</v>
+      </c>
+      <c r="M192" t="n">
+        <v>0</v>
+      </c>
+      <c r="N192" t="n">
+        <v>1</v>
+      </c>
+      <c r="O192" t="n">
+        <v>440</v>
+      </c>
+      <c r="P192" t="inlineStr">
+        <is>
+          <t>Correspondence of Logan Cole Respecting Dungeon Bashing</t>
+        </is>
+      </c>
+      <c r="Q192" t="inlineStr">
+        <is>
+          <t>Cynesige Nottley</t>
+        </is>
+      </c>
+      <c r="S192" s="13" t="inlineStr">
+        <is>
+          <t>Προστεθῇ ἃς παράλληλοί ἡμικυκλίου συστήσασθαι· εἰς ιθ΄ ἐστιν ἔχον παραλληλόγραμμον ἐμπίπτουσα πέρατα</t>
+        </is>
+      </c>
+      <c r="T192" t="n">
+        <v>6</v>
+      </c>
+      <c r="U192" t="n">
+        <v>6</v>
+      </c>
+      <c r="V192" t="n">
+        <v>36</v>
+      </c>
+      <c r="W192" t="n">
+        <v>149</v>
+      </c>
+      <c r="X192" t="n">
+        <v>143</v>
+      </c>
+      <c r="Y192" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="AB192" t="inlineStr">
+        <is>
+          <t>Cynesige Nottley</t>
+        </is>
+      </c>
+      <c r="AC192" t="inlineStr">
+        <is>
+          <t>_names_anglo_saxon_surnames</t>
+        </is>
+      </c>
+      <c r="AE192" t="inlineStr">
+        <is>
+          <t>Female</t>
+        </is>
+      </c>
+      <c r="AJ192" t="n">
+        <v>0.06</v>
+      </c>
+      <c r="AK192" t="inlineStr">
+        <is>
+          <t>{communication} of {person_1} {conjunction_about} {topic}</t>
+        </is>
+      </c>
+      <c r="AL192" t="inlineStr">
+        <is>
+          <t>Dungeon Bashing</t>
+        </is>
+      </c>
+      <c r="AM192" t="n">
+        <v>0.39</v>
+      </c>
+      <c r="AN192" t="n">
+        <v>390</v>
+      </c>
+      <c r="AO192" t="n">
+        <v>1</v>
+      </c>
+      <c r="AP192" t="n">
+        <v>50</v>
+      </c>
+      <c r="AQ192" t="n">
+        <v>0</v>
+      </c>
+      <c r="AR192" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS192" t="n">
+        <v>0</v>
+      </c>
+      <c r="AT192" t="n">
+        <v>0</v>
+      </c>
+      <c r="AU192" t="b">
+        <v>0</v>
+      </c>
+      <c r="AV192" t="inlineStr">
+        <is>
+          <t>Standard</t>
+        </is>
+      </c>
+      <c r="AW192" t="inlineStr">
+        <is>
+          <t>ed775fdd-737c-4c3d-a8a7-0380f32633e7</t>
+        </is>
+      </c>
+      <c r="AX192" t="inlineStr">
+        <is>
+          <t>has_been_archived</t>
+        </is>
+      </c>
+    </row>
+    <row r="193">
+      <c r="A193" t="inlineStr">
+        <is>
+          <t>Codex</t>
+        </is>
+      </c>
+      <c r="B193" t="inlineStr">
+        <is>
+          <t>Parchment</t>
+        </is>
+      </c>
+      <c r="C193" t="n">
+        <v>2</v>
+      </c>
+      <c r="D193" t="n">
+        <v>1000</v>
+      </c>
+      <c r="E193" t="n">
+        <v>63</v>
+      </c>
+      <c r="F193" t="inlineStr">
+        <is>
+          <t>Regional</t>
+        </is>
+      </c>
+      <c r="G193" t="inlineStr">
+        <is>
+          <t>Common</t>
+        </is>
+      </c>
+      <c r="H193" t="inlineStr">
+        <is>
+          <t>Knowledge (architecture)</t>
+        </is>
+      </c>
+      <c r="I193" t="inlineStr">
+        <is>
+          <t>Knowledge (architecture)</t>
+        </is>
+      </c>
+      <c r="J193" t="n">
+        <v>3</v>
+      </c>
+      <c r="K193" t="n">
+        <v>0</v>
+      </c>
+      <c r="L193" t="n">
+        <v>3</v>
+      </c>
+      <c r="M193" t="n">
+        <v>0</v>
+      </c>
+      <c r="N193" t="n">
+        <v>1</v>
+      </c>
+      <c r="O193" t="n">
+        <v>410</v>
+      </c>
+      <c r="P193" t="inlineStr">
+        <is>
+          <t>Ruminations in Architecture</t>
+        </is>
+      </c>
+      <c r="Q193" t="inlineStr">
+        <is>
+          <t>The Gracious Mégane Dubuisson-Lebon</t>
+        </is>
+      </c>
+      <c r="R193" t="inlineStr">
+        <is>
+          <t>The Honorable Muriel Henin</t>
+        </is>
+      </c>
+      <c r="S193" s="13" t="inlineStr">
+        <is>
+          <t>Λγ΄ ιβ΄ ἐπιφανείας ἀλλήλοις τριγώνῳ κθ΄</t>
+        </is>
+      </c>
+      <c r="T193" t="n">
+        <v>6</v>
+      </c>
+      <c r="U193" t="n">
+        <v>6</v>
+      </c>
+      <c r="V193" t="n">
+        <v>92</v>
+      </c>
+      <c r="W193" t="n">
+        <v>578</v>
+      </c>
+      <c r="X193" t="n">
+        <v>576</v>
+      </c>
+      <c r="Y193" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="AB193" t="inlineStr">
+        <is>
+          <t>Mégane Dubuisson-Lebon</t>
+        </is>
+      </c>
+      <c r="AC193" t="inlineStr">
+        <is>
+          <t>_names_french_surnames</t>
+        </is>
+      </c>
+      <c r="AD193" t="inlineStr">
+        <is>
+          <t>The Gracious</t>
+        </is>
+      </c>
+      <c r="AE193" t="inlineStr">
+        <is>
+          <t>Female</t>
+        </is>
+      </c>
+      <c r="AF193" t="inlineStr">
+        <is>
+          <t>Muriel Henin</t>
+        </is>
+      </c>
+      <c r="AG193" t="inlineStr">
+        <is>
+          <t>_names_french_surnames</t>
+        </is>
+      </c>
+      <c r="AH193" t="inlineStr">
+        <is>
+          <t>Female</t>
+        </is>
+      </c>
+      <c r="AI193" t="inlineStr">
+        <is>
+          <t>The Honorable</t>
+        </is>
+      </c>
+      <c r="AJ193" t="n">
+        <v>0.06</v>
+      </c>
+      <c r="AK193" t="inlineStr">
+        <is>
+          <t>{study_in} in {topic}</t>
+        </is>
+      </c>
+      <c r="AL193" t="inlineStr">
+        <is>
+          <t>Architecture</t>
+        </is>
+      </c>
+      <c r="AM193" t="n">
+        <v>0.37</v>
+      </c>
+      <c r="AN193" t="n">
+        <v>370</v>
+      </c>
+      <c r="AO193" t="n">
+        <v>4</v>
+      </c>
+      <c r="AP193" t="n">
+        <v>40</v>
+      </c>
+      <c r="AQ193" t="n">
+        <v>0</v>
+      </c>
+      <c r="AR193" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS193" t="n">
+        <v>0</v>
+      </c>
+      <c r="AT193" t="n">
+        <v>0</v>
+      </c>
+      <c r="AU193" t="b">
+        <v>1</v>
+      </c>
+      <c r="AV193" t="inlineStr">
+        <is>
+          <t>Standard</t>
+        </is>
+      </c>
+      <c r="AW193" t="inlineStr">
+        <is>
+          <t>f6fbba70-0604-447f-84b6-9e973d123fcc</t>
+        </is>
+      </c>
+      <c r="AX193" t="inlineStr">
+        <is>
+          <t>has_been_archived</t>
+        </is>
+      </c>
+    </row>
+    <row r="194">
+      <c r="A194" t="inlineStr">
+        <is>
+          <t>Codex</t>
+        </is>
+      </c>
+      <c r="B194" t="inlineStr">
+        <is>
+          <t>Vellum</t>
+        </is>
+      </c>
+      <c r="C194" t="n">
+        <v>2</v>
+      </c>
+      <c r="D194" t="n">
+        <v>800</v>
+      </c>
+      <c r="E194" t="n">
+        <v>51</v>
+      </c>
+      <c r="F194" t="inlineStr">
+        <is>
+          <t>Common</t>
+        </is>
+      </c>
+      <c r="H194" t="inlineStr">
+        <is>
+          <t>Craft (tanning)</t>
+        </is>
+      </c>
+      <c r="I194" t="inlineStr">
+        <is>
+          <t>Craft (tanning)</t>
+        </is>
+      </c>
+      <c r="J194" t="n">
+        <v>4</v>
+      </c>
+      <c r="K194" t="n">
+        <v>0</v>
+      </c>
+      <c r="L194" t="n">
+        <v>5</v>
+      </c>
+      <c r="M194" t="n">
+        <v>0</v>
+      </c>
+      <c r="N194" t="n">
+        <v>1</v>
+      </c>
+      <c r="O194" t="n">
+        <v>2812</v>
+      </c>
+      <c r="P194" t="inlineStr">
+        <is>
+          <t>Life of The Temptress with emphasis upon Tanning</t>
+        </is>
+      </c>
+      <c r="Q194" t="inlineStr">
+        <is>
+          <t>Axel Choquet</t>
+        </is>
+      </c>
+      <c r="S194" s="13" t="inlineStr">
+        <is>
+          <t>Life of The Temptress with emphasis upon Tanning</t>
+        </is>
+      </c>
+      <c r="T194" t="n">
+        <v>5</v>
+      </c>
+      <c r="U194" t="n">
+        <v>5</v>
+      </c>
+      <c r="V194" t="n">
+        <v>343</v>
+      </c>
+      <c r="W194" t="n">
+        <v>47</v>
+      </c>
+      <c r="X194" t="n">
+        <v>46</v>
+      </c>
+      <c r="Y194" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="AB194" t="inlineStr">
+        <is>
+          <t>Axel Choquet</t>
+        </is>
+      </c>
+      <c r="AC194" t="inlineStr">
+        <is>
+          <t>_names_french_surnames</t>
+        </is>
+      </c>
+      <c r="AE194" t="inlineStr">
+        <is>
+          <t>Male</t>
+        </is>
+      </c>
+      <c r="AJ194" t="n">
+        <v>0.06</v>
+      </c>
+      <c r="AK194" t="inlineStr">
+        <is>
+          <t>{biography_starter} of {person_evil} with emphasis upon {topic}</t>
+        </is>
+      </c>
+      <c r="AL194" t="inlineStr">
+        <is>
+          <t>Tanning</t>
+        </is>
+      </c>
+      <c r="AM194" t="n">
+        <v>0.39</v>
+      </c>
+      <c r="AN194" t="n">
+        <v>312</v>
+      </c>
+      <c r="AO194" t="n">
+        <v>12.5</v>
+      </c>
+      <c r="AP194" t="n">
+        <v>2500</v>
+      </c>
+      <c r="AQ194" t="n">
+        <v>0</v>
+      </c>
+      <c r="AR194" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS194" t="n">
+        <v>0</v>
+      </c>
+      <c r="AT194" t="n">
+        <v>0</v>
+      </c>
+      <c r="AU194" t="b">
+        <v>0</v>
+      </c>
+      <c r="AV194" t="inlineStr">
+        <is>
+          <t>Standard</t>
+        </is>
+      </c>
+      <c r="AW194" t="inlineStr">
+        <is>
+          <t>30506752-49cb-4f73-b4ad-32e2eb5b4dce</t>
+        </is>
+      </c>
+      <c r="AX194" t="inlineStr">
+        <is>
+          <t>has_been_archived</t>
+        </is>
+      </c>
+    </row>
+    <row r="195">
+      <c r="A195" t="inlineStr">
+        <is>
+          <t>Codex</t>
+        </is>
+      </c>
+      <c r="B195" t="inlineStr">
+        <is>
+          <t>Parchment</t>
+        </is>
+      </c>
+      <c r="C195" t="n">
+        <v>1</v>
+      </c>
+      <c r="D195" t="n">
+        <v>600</v>
+      </c>
+      <c r="E195" t="n">
+        <v>38</v>
+      </c>
+      <c r="F195" t="inlineStr">
+        <is>
+          <t>Regional</t>
+        </is>
+      </c>
+      <c r="H195" t="inlineStr">
+        <is>
+          <t>Manual of Arms</t>
+        </is>
+      </c>
+      <c r="I195" t="inlineStr">
+        <is>
+          <t>Manual of Arms</t>
+        </is>
+      </c>
+      <c r="J195" t="n">
+        <v>3</v>
+      </c>
+      <c r="K195" t="n">
+        <v>0</v>
+      </c>
+      <c r="L195" t="n">
+        <v>5</v>
+      </c>
+      <c r="M195" t="n">
+        <v>0</v>
+      </c>
+      <c r="N195" t="n">
+        <v>1</v>
+      </c>
+      <c r="O195" t="n">
+        <v>1806</v>
+      </c>
+      <c r="P195" t="inlineStr">
+        <is>
+          <t>The Evil of Nazaire Reverdin, on the Subject of Manual of Arms</t>
+        </is>
+      </c>
+      <c r="Q195" t="inlineStr">
+        <is>
+          <t>Croydon Simpson the Lazy</t>
+        </is>
+      </c>
+      <c r="S195" s="13" t="inlineStr">
+        <is>
+          <t>Ἡμικυκλίου γωνίαι σκαληνὸν ἴσας αὐτῇ ἔχῃ ῥομβοειδὲς ἀνίσων γωνία εὐθυγράμμῳ μηδέτερα</t>
+        </is>
+      </c>
+      <c r="T195" t="n">
+        <v>4</v>
+      </c>
+      <c r="U195" t="n">
+        <v>4</v>
+      </c>
+      <c r="V195" t="n">
+        <v>44</v>
+      </c>
+      <c r="W195" t="n">
+        <v>6</v>
+      </c>
+      <c r="X195" t="n">
+        <v>5</v>
+      </c>
+      <c r="Y195" t="n">
+        <v>0.33</v>
+      </c>
+      <c r="AA195" t="inlineStr">
+        <is>
+          <t>the Lazy</t>
+        </is>
+      </c>
+      <c r="AB195" t="inlineStr">
+        <is>
+          <t>Croydon Simpson</t>
+        </is>
+      </c>
+      <c r="AC195" t="inlineStr">
+        <is>
+          <t>_names_english_surnames</t>
+        </is>
+      </c>
+      <c r="AE195" t="inlineStr">
+        <is>
+          <t>Male</t>
+        </is>
+      </c>
+      <c r="AJ195" t="n">
+        <v>0.06</v>
+      </c>
+      <c r="AK195" t="inlineStr">
+        <is>
+          <t>{the_1} {negative_1} of {person_1}, on the Subject of {topic}</t>
+        </is>
+      </c>
+      <c r="AL195" t="inlineStr">
+        <is>
+          <t>Manual of Arms</t>
+        </is>
+      </c>
+      <c r="AM195" t="n">
+        <v>0.37</v>
+      </c>
+      <c r="AN195" t="n">
+        <v>222</v>
+      </c>
+      <c r="AO195" t="n">
+        <v>8</v>
+      </c>
+      <c r="AP195" t="n">
+        <v>1584</v>
+      </c>
+      <c r="AQ195" t="n">
+        <v>0</v>
+      </c>
+      <c r="AR195" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS195" t="n">
+        <v>0</v>
+      </c>
+      <c r="AT195" t="n">
+        <v>0</v>
+      </c>
+      <c r="AU195" t="b">
+        <v>0</v>
+      </c>
+      <c r="AV195" t="inlineStr">
+        <is>
+          <t>Standard</t>
+        </is>
+      </c>
+      <c r="AW195" t="inlineStr">
+        <is>
+          <t>630df438-5839-435f-a6f2-c0ddbcb559b9</t>
+        </is>
+      </c>
+      <c r="AX195" t="inlineStr">
+        <is>
+          <t>has_been_archived</t>
+        </is>
+      </c>
+    </row>
+    <row r="196">
+      <c r="A196" t="inlineStr">
+        <is>
+          <t>Codex</t>
+        </is>
+      </c>
+      <c r="B196" t="inlineStr">
+        <is>
+          <t>Vellum</t>
+        </is>
+      </c>
+      <c r="C196" t="n">
+        <v>2</v>
+      </c>
+      <c r="D196" t="n">
+        <v>320</v>
+      </c>
+      <c r="E196" t="n">
+        <v>21</v>
+      </c>
+      <c r="F196" t="inlineStr">
+        <is>
+          <t>Classical</t>
+        </is>
+      </c>
+      <c r="H196" t="inlineStr">
+        <is>
+          <t>Esoteric: Black Lore of Zahar</t>
+        </is>
+      </c>
+      <c r="I196" t="inlineStr">
+        <is>
+          <t>Riding</t>
+        </is>
+      </c>
+      <c r="J196" t="n">
+        <v>0.32</v>
+      </c>
+      <c r="K196" t="n">
+        <v>1</v>
+      </c>
+      <c r="L196" t="n">
+        <v>1</v>
+      </c>
+      <c r="M196" t="n">
+        <v>1</v>
+      </c>
+      <c r="N196" t="n">
+        <v>0.32</v>
+      </c>
+      <c r="O196" t="n">
+        <v>2320</v>
+      </c>
+      <c r="P196" t="inlineStr">
+        <is>
+          <t>Mathilde Tassel and Guilt: Aspects of Riding</t>
+        </is>
+      </c>
+      <c r="Q196" t="inlineStr">
+        <is>
+          <t>Eardwulf Beeston</t>
+        </is>
+      </c>
+      <c r="S196" s="13" t="inlineStr">
+        <is>
+          <t>Praetore obsidibus impetum contrahere factum</t>
+        </is>
+      </c>
+      <c r="T196" t="n">
+        <v>2</v>
+      </c>
+      <c r="U196" t="n">
+        <v>2</v>
+      </c>
+      <c r="V196" t="n">
+        <v>369</v>
+      </c>
+      <c r="W196" t="n">
+        <v>19</v>
+      </c>
+      <c r="X196" t="n">
+        <v>18</v>
+      </c>
+      <c r="Y196" t="n">
+        <v>0.33</v>
+      </c>
+      <c r="AB196" t="inlineStr">
+        <is>
+          <t>Eardwulf Beeston</t>
+        </is>
+      </c>
+      <c r="AC196" t="inlineStr">
+        <is>
+          <t>_names_anglo_saxon_surnames</t>
+        </is>
+      </c>
+      <c r="AE196" t="inlineStr">
+        <is>
+          <t>Male</t>
+        </is>
+      </c>
+      <c r="AJ196" t="n">
+        <v>0.06</v>
+      </c>
+      <c r="AK196" t="inlineStr">
+        <is>
+          <t>{person_1} and {negative_1}: Aspects of {topic}</t>
+        </is>
+      </c>
+      <c r="AL196" t="inlineStr">
+        <is>
+          <t>Riding</t>
+        </is>
+      </c>
+      <c r="AM196" t="n">
+        <v>0.39</v>
+      </c>
+      <c r="AN196" t="n">
+        <v>390</v>
+      </c>
+      <c r="AO196" t="n">
+        <v>1</v>
+      </c>
+      <c r="AP196" t="n">
+        <v>330</v>
+      </c>
+      <c r="AQ196" t="n">
+        <v>1</v>
+      </c>
+      <c r="AR196" t="n">
+        <v>1600</v>
+      </c>
+      <c r="AS196" t="n">
+        <v>0</v>
+      </c>
+      <c r="AT196" t="n">
+        <v>0</v>
+      </c>
+      <c r="AU196" t="b">
+        <v>0</v>
+      </c>
+      <c r="AV196" t="inlineStr">
+        <is>
+          <t>Standard</t>
+        </is>
+      </c>
+      <c r="AW196" t="inlineStr">
+        <is>
+          <t>82759e53-c398-480a-99de-abdbd72b06c7</t>
+        </is>
+      </c>
+      <c r="AX196" t="inlineStr">
+        <is>
+          <t>has_been_archived</t>
+        </is>
+      </c>
+    </row>
+    <row r="197">
+      <c r="A197" t="inlineStr">
+        <is>
+          <t>Codex</t>
+        </is>
+      </c>
+      <c r="B197" t="inlineStr">
+        <is>
+          <t>Parchment</t>
+        </is>
+      </c>
+      <c r="C197" t="n">
+        <v>1</v>
+      </c>
+      <c r="D197" t="n">
+        <v>500</v>
+      </c>
+      <c r="E197" t="n">
+        <v>32</v>
+      </c>
+      <c r="F197" t="inlineStr">
+        <is>
+          <t>Common</t>
+        </is>
+      </c>
+      <c r="H197" t="inlineStr">
+        <is>
+          <t>Craft (weaponsmithing)</t>
+        </is>
+      </c>
+      <c r="I197" t="inlineStr">
+        <is>
+          <t>Craft (weaponsmithing)</t>
+        </is>
+      </c>
+      <c r="J197" t="n">
+        <v>1</v>
+      </c>
+      <c r="K197" t="n">
+        <v>0</v>
+      </c>
+      <c r="L197" t="n">
+        <v>2</v>
+      </c>
+      <c r="M197" t="n">
+        <v>0</v>
+      </c>
+      <c r="N197" t="n">
+        <v>1</v>
+      </c>
+      <c r="O197" t="n">
+        <v>810</v>
+      </c>
+      <c r="P197" t="inlineStr">
+        <is>
+          <t>The Jovial Revelation: Weaponsmithing</t>
+        </is>
+      </c>
+      <c r="Q197" t="inlineStr">
+        <is>
+          <t>Mister Andvaranaut Johnsen</t>
+        </is>
+      </c>
+      <c r="S197" s="13" t="inlineStr">
+        <is>
+          <t>The Jovial Revelation: Weaponsmithing</t>
+        </is>
+      </c>
+      <c r="T197" t="n">
+        <v>3</v>
+      </c>
+      <c r="U197" t="n">
+        <v>3</v>
+      </c>
+      <c r="V197" t="n">
+        <v>9</v>
+      </c>
+      <c r="W197" t="n">
+        <v>1</v>
+      </c>
+      <c r="X197" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y197" t="n">
+        <v>1</v>
+      </c>
+      <c r="AB197" t="inlineStr">
+        <is>
+          <t>Andvaranaut Johnsen</t>
+        </is>
+      </c>
+      <c r="AC197" t="inlineStr">
+        <is>
+          <t>_names_norse_surnames_male</t>
+        </is>
+      </c>
+      <c r="AD197" t="inlineStr">
+        <is>
+          <t>Mister</t>
+        </is>
+      </c>
+      <c r="AE197" t="inlineStr">
+        <is>
+          <t>Male</t>
+        </is>
+      </c>
+      <c r="AJ197" t="n">
+        <v>0.06</v>
+      </c>
+      <c r="AK197" t="inlineStr">
+        <is>
+          <t>The {adjective_1} {noun_1}: {topic}</t>
+        </is>
+      </c>
+      <c r="AL197" t="inlineStr">
+        <is>
+          <t>Weaponsmithing</t>
+        </is>
+      </c>
+      <c r="AM197" t="n">
+        <v>0.37</v>
+      </c>
+      <c r="AN197" t="n">
+        <v>185</v>
+      </c>
+      <c r="AO197" t="n">
+        <v>1.25</v>
+      </c>
+      <c r="AP197" t="n">
+        <v>625</v>
+      </c>
+      <c r="AQ197" t="n">
+        <v>0</v>
+      </c>
+      <c r="AR197" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS197" t="n">
+        <v>0</v>
+      </c>
+      <c r="AT197" t="n">
+        <v>0</v>
+      </c>
+      <c r="AU197" t="b">
+        <v>0</v>
+      </c>
+      <c r="AV197" t="inlineStr">
+        <is>
+          <t>Standard</t>
+        </is>
+      </c>
+      <c r="AW197" t="inlineStr">
+        <is>
+          <t>5613ca72-a734-4ea2-ab1d-d54a83c669ef</t>
+        </is>
+      </c>
+      <c r="AX197" t="inlineStr">
+        <is>
+          <t>has_been_archived</t>
+        </is>
+      </c>
+    </row>
+    <row r="198">
+      <c r="A198" t="inlineStr">
+        <is>
+          <t>Codex</t>
+        </is>
+      </c>
+      <c r="B198" t="inlineStr">
+        <is>
+          <t>Vellum</t>
+        </is>
+      </c>
+      <c r="C198" t="n">
+        <v>2</v>
+      </c>
+      <c r="D198" t="n">
+        <v>1000</v>
+      </c>
+      <c r="E198" t="n">
+        <v>63</v>
+      </c>
+      <c r="F198" t="inlineStr">
+        <is>
+          <t>Classical</t>
+        </is>
+      </c>
+      <c r="H198" t="inlineStr">
+        <is>
+          <t>Land Surveying</t>
+        </is>
+      </c>
+      <c r="I198" t="inlineStr">
+        <is>
+          <t>Land Surveying</t>
+        </is>
+      </c>
+      <c r="J198" t="n">
+        <v>1</v>
+      </c>
+      <c r="K198" t="n">
+        <v>0</v>
+      </c>
+      <c r="L198" t="n">
+        <v>1</v>
+      </c>
+      <c r="M198" t="n">
+        <v>0</v>
+      </c>
+      <c r="N198" t="n">
+        <v>1</v>
+      </c>
+      <c r="O198" t="n">
+        <v>890</v>
+      </c>
+      <c r="P198" t="inlineStr">
+        <is>
+          <t>Abstractions in Land Surveying</t>
+        </is>
+      </c>
+      <c r="Q198" t="inlineStr">
+        <is>
+          <t>Mistress Perrine Fraisse the Horrible</t>
+        </is>
+      </c>
+      <c r="S198" s="13" t="inlineStr">
+        <is>
+          <t>Lapides agendos voluntate medio persuadent traduxisse reductos tulingos nobis pervenerant</t>
+        </is>
+      </c>
+      <c r="T198" t="n">
+        <v>6</v>
+      </c>
+      <c r="U198" t="n">
+        <v>6</v>
+      </c>
+      <c r="V198" t="n">
+        <v>31</v>
+      </c>
+      <c r="W198" t="n">
+        <v>4</v>
+      </c>
+      <c r="X198" t="n">
+        <v>2</v>
+      </c>
+      <c r="Y198" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="AA198" t="inlineStr">
+        <is>
+          <t>the Horrible</t>
+        </is>
+      </c>
+      <c r="AB198" t="inlineStr">
+        <is>
+          <t>Perrine Fraisse</t>
+        </is>
+      </c>
+      <c r="AC198" t="inlineStr">
+        <is>
+          <t>_names_french_surnames</t>
+        </is>
+      </c>
+      <c r="AD198" t="inlineStr">
+        <is>
+          <t>Mistress</t>
+        </is>
+      </c>
+      <c r="AE198" t="inlineStr">
+        <is>
+          <t>Female</t>
+        </is>
+      </c>
+      <c r="AJ198" t="n">
+        <v>0.06</v>
+      </c>
+      <c r="AK198" t="inlineStr">
+        <is>
+          <t>{study_in} in {topic}</t>
+        </is>
+      </c>
+      <c r="AL198" t="inlineStr">
+        <is>
+          <t>Land Surveying</t>
+        </is>
+      </c>
+      <c r="AM198" t="n">
+        <v>0.39</v>
+      </c>
+      <c r="AN198" t="n">
+        <v>390</v>
+      </c>
+      <c r="AO198" t="n">
+        <v>1</v>
+      </c>
+      <c r="AP198" t="n">
+        <v>500</v>
+      </c>
+      <c r="AQ198" t="n">
+        <v>0</v>
+      </c>
+      <c r="AR198" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS198" t="n">
+        <v>0</v>
+      </c>
+      <c r="AT198" t="n">
+        <v>0</v>
+      </c>
+      <c r="AU198" t="b">
+        <v>0</v>
+      </c>
+      <c r="AV198" t="inlineStr">
+        <is>
+          <t>Standard</t>
+        </is>
+      </c>
+      <c r="AW198" t="inlineStr">
+        <is>
+          <t>a1fa192b-ea10-4d5c-a753-b45508ed9ee0</t>
+        </is>
+      </c>
+      <c r="AX198" t="inlineStr">
+        <is>
+          <t>has_been_archived</t>
+        </is>
+      </c>
+    </row>
+    <row r="199">
+      <c r="A199" t="inlineStr">
+        <is>
+          <t>Codex</t>
+        </is>
+      </c>
+      <c r="B199" t="inlineStr">
+        <is>
+          <t>Parchment</t>
+        </is>
+      </c>
+      <c r="C199" t="n">
+        <v>1</v>
+      </c>
+      <c r="D199" t="n">
+        <v>500</v>
+      </c>
+      <c r="E199" t="n">
+        <v>32</v>
+      </c>
+      <c r="F199" t="inlineStr">
+        <is>
+          <t>Common</t>
+        </is>
+      </c>
+      <c r="H199" t="inlineStr">
+        <is>
+          <t>Performance (playing instruments)</t>
+        </is>
+      </c>
+      <c r="I199" t="inlineStr">
+        <is>
+          <t>Performance (playing instruments)</t>
+        </is>
+      </c>
+      <c r="J199" t="n">
+        <v>2</v>
+      </c>
+      <c r="K199" t="n">
+        <v>0</v>
+      </c>
+      <c r="L199" t="n">
+        <v>4</v>
+      </c>
+      <c r="M199" t="n">
+        <v>0</v>
+      </c>
+      <c r="N199" t="n">
+        <v>1</v>
+      </c>
+      <c r="O199" t="n">
+        <v>685</v>
+      </c>
+      <c r="P199" t="inlineStr">
+        <is>
+          <t>Meditation on The Floote and Its Ability to Attract Maidens Fair</t>
+        </is>
+      </c>
+      <c r="Q199" t="inlineStr">
+        <is>
+          <t>Sarah Shakir</t>
+        </is>
+      </c>
+      <c r="S199" s="13" t="inlineStr">
+        <is>
+          <t>Meditation on The Floote and Its Ability to Attract Maidens Fair</t>
+        </is>
+      </c>
+      <c r="T199" t="n">
+        <v>3</v>
+      </c>
+      <c r="U199" t="n">
+        <v>3</v>
+      </c>
+      <c r="V199" t="n">
+        <v>71</v>
+      </c>
+      <c r="W199" t="n">
+        <v>31</v>
+      </c>
+      <c r="X199" t="n">
+        <v>30</v>
+      </c>
+      <c r="Y199" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="AB199" t="inlineStr">
+        <is>
+          <t>Sarah Shakir</t>
+        </is>
+      </c>
+      <c r="AC199" t="inlineStr">
+        <is>
+          <t>_names_arabic_surnames</t>
+        </is>
+      </c>
+      <c r="AE199" t="inlineStr">
+        <is>
+          <t>Female</t>
+        </is>
+      </c>
+      <c r="AJ199" t="n">
+        <v>0.06</v>
+      </c>
+      <c r="AK199" t="inlineStr">
+        <is>
+          <t>{study_on} on {topic}</t>
+        </is>
+      </c>
+      <c r="AL199" t="inlineStr">
+        <is>
+          <t>The Floote and Its Ability to Attract Maidens Fair</t>
+        </is>
+      </c>
+      <c r="AM199" t="n">
+        <v>0.37</v>
+      </c>
+      <c r="AN199" t="n">
+        <v>185</v>
+      </c>
+      <c r="AO199" t="n">
+        <v>4</v>
+      </c>
+      <c r="AP199" t="n">
+        <v>500</v>
+      </c>
+      <c r="AQ199" t="n">
+        <v>0</v>
+      </c>
+      <c r="AR199" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS199" t="n">
+        <v>0</v>
+      </c>
+      <c r="AT199" t="n">
+        <v>0</v>
+      </c>
+      <c r="AU199" t="b">
+        <v>0</v>
+      </c>
+      <c r="AV199" t="inlineStr">
+        <is>
+          <t>Standard</t>
+        </is>
+      </c>
+      <c r="AW199" t="inlineStr">
+        <is>
+          <t>ee2e8cee-7e21-43bb-a5dc-ca9456801915</t>
+        </is>
+      </c>
+      <c r="AX199" t="inlineStr">
+        <is>
+          <t>has_been_archived</t>
+        </is>
+      </c>
+    </row>
+    <row r="200">
+      <c r="A200" t="inlineStr">
+        <is>
+          <t>Codex</t>
+        </is>
+      </c>
+      <c r="B200" t="inlineStr">
+        <is>
+          <t>Parchment</t>
+        </is>
+      </c>
+      <c r="C200" t="n">
+        <v>1</v>
+      </c>
+      <c r="D200" t="n">
+        <v>334</v>
+      </c>
+      <c r="E200" t="n">
+        <v>23</v>
+      </c>
+      <c r="F200" t="inlineStr">
+        <is>
+          <t>Classical</t>
+        </is>
+      </c>
+      <c r="H200" t="inlineStr">
+        <is>
+          <t>Manual of Arms</t>
+        </is>
+      </c>
+      <c r="I200" t="inlineStr">
+        <is>
+          <t>Manual of Arms</t>
+        </is>
+      </c>
+      <c r="J200" t="n">
+        <v>1</v>
+      </c>
+      <c r="K200" t="n">
+        <v>0</v>
+      </c>
+      <c r="L200" t="n">
+        <v>3</v>
+      </c>
+      <c r="M200" t="n">
+        <v>0</v>
+      </c>
+      <c r="N200" t="n">
+        <v>1</v>
+      </c>
+      <c r="O200" t="n">
+        <v>191</v>
+      </c>
+      <c r="P200" t="inlineStr">
+        <is>
+          <t>Examination in Manual of Arms</t>
+        </is>
+      </c>
+      <c r="Q200" t="inlineStr">
+        <is>
+          <t>Aurelius Faminia</t>
+        </is>
+      </c>
+      <c r="S200" s="13" t="inlineStr">
+        <is>
+          <t>Iamque enuntiarentur posset? annuus continuos praeterita romano consecuti lacrimas</t>
+        </is>
+      </c>
+      <c r="T200" t="n">
+        <v>2</v>
+      </c>
+      <c r="U200" t="n">
+        <v>2</v>
+      </c>
+      <c r="V200" t="n">
+        <v>56</v>
+      </c>
+      <c r="W200" t="n">
+        <v>98</v>
+      </c>
+      <c r="X200" t="n">
+        <v>94</v>
+      </c>
+      <c r="Y200" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="AB200" t="inlineStr">
+        <is>
+          <t>Aurelius Faminia</t>
+        </is>
+      </c>
+      <c r="AC200" t="inlineStr">
+        <is>
+          <t>_names_roman_surnames</t>
+        </is>
+      </c>
+      <c r="AE200" t="inlineStr">
+        <is>
+          <t>Male</t>
+        </is>
+      </c>
+      <c r="AJ200" t="n">
+        <v>0.06</v>
+      </c>
+      <c r="AK200" t="inlineStr">
+        <is>
+          <t>{study_in} in {topic}</t>
+        </is>
+      </c>
+      <c r="AL200" t="inlineStr">
+        <is>
+          <t>Manual of Arms</t>
+        </is>
+      </c>
+      <c r="AM200" t="n">
+        <v>0.37</v>
+      </c>
+      <c r="AN200" t="n">
+        <v>124</v>
+      </c>
+      <c r="AO200" t="n">
+        <v>2</v>
+      </c>
+      <c r="AP200" t="n">
+        <v>67</v>
+      </c>
+      <c r="AQ200" t="n">
+        <v>0</v>
+      </c>
+      <c r="AR200" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS200" t="n">
+        <v>0</v>
+      </c>
+      <c r="AT200" t="n">
+        <v>0</v>
+      </c>
+      <c r="AU200" t="b">
+        <v>0</v>
+      </c>
+      <c r="AV200" t="inlineStr">
+        <is>
+          <t>Standard</t>
+        </is>
+      </c>
+      <c r="AW200" t="inlineStr">
+        <is>
+          <t>9ccbbd40-955d-41ec-a160-f487bba2d8fe</t>
+        </is>
+      </c>
+      <c r="AX200" t="inlineStr">
+        <is>
+          <t>has_been_archived</t>
+        </is>
+      </c>
+    </row>
+    <row r="201">
+      <c r="A201" t="inlineStr">
+        <is>
+          <t>Codex</t>
+        </is>
+      </c>
+      <c r="B201" t="inlineStr">
+        <is>
+          <t>Parchment</t>
+        </is>
+      </c>
+      <c r="C201" t="n">
+        <v>1</v>
+      </c>
+      <c r="D201" t="n">
+        <v>500</v>
+      </c>
+      <c r="E201" t="n">
+        <v>32</v>
+      </c>
+      <c r="F201" t="inlineStr">
+        <is>
+          <t>Common</t>
+        </is>
+      </c>
+      <c r="H201" t="inlineStr">
+        <is>
+          <t>Animal Husbandry</t>
+        </is>
+      </c>
+      <c r="I201" t="inlineStr">
+        <is>
+          <t>Animal Husbandry</t>
+        </is>
+      </c>
+      <c r="J201" t="n">
+        <v>1</v>
+      </c>
+      <c r="K201" t="n">
+        <v>0</v>
+      </c>
+      <c r="L201" t="n">
+        <v>2</v>
+      </c>
+      <c r="M201" t="n">
+        <v>0</v>
+      </c>
+      <c r="N201" t="n">
+        <v>1</v>
+      </c>
+      <c r="O201" t="n">
+        <v>185</v>
+      </c>
+      <c r="P201" t="inlineStr">
+        <is>
+          <t>The Impenetrable Sojourn of Abhorrence: Animal Husbandry</t>
+        </is>
+      </c>
+      <c r="Q201" t="inlineStr">
+        <is>
+          <t>Wærmund Goodwin</t>
+        </is>
+      </c>
+      <c r="S201" s="13" t="inlineStr">
+        <is>
+          <t>The Impenetrable Sojourn of Abhorrence: Animal Husbandry</t>
+        </is>
+      </c>
+      <c r="T201" t="n">
+        <v>3</v>
+      </c>
+      <c r="U201" t="n">
+        <v>3</v>
+      </c>
+      <c r="V201" t="n">
+        <v>49</v>
+      </c>
+      <c r="W201" t="n">
+        <v>1704</v>
+      </c>
+      <c r="X201" t="n">
+        <v>1703</v>
+      </c>
+      <c r="Y201" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB201" t="inlineStr">
+        <is>
+          <t>Wærmund Goodwin</t>
+        </is>
+      </c>
+      <c r="AC201" t="inlineStr">
+        <is>
+          <t>_names_anglo_saxon_surnames</t>
+        </is>
+      </c>
+      <c r="AE201" t="inlineStr">
+        <is>
+          <t>Male</t>
+        </is>
+      </c>
+      <c r="AJ201" t="n">
+        <v>0.06</v>
+      </c>
+      <c r="AK201" t="inlineStr">
+        <is>
+          <t>The {adjective_1} {noun_1} of {noun_2}: {topic}</t>
+        </is>
+      </c>
+      <c r="AL201" t="inlineStr">
+        <is>
+          <t>Animal Husbandry</t>
+        </is>
+      </c>
+      <c r="AM201" t="n">
+        <v>0.37</v>
+      </c>
+      <c r="AN201" t="n">
+        <v>185</v>
+      </c>
+      <c r="AO201" t="n">
+        <v>1.25</v>
+      </c>
+      <c r="AP201" t="n">
+        <v>0</v>
+      </c>
+      <c r="AQ201" t="n">
+        <v>0</v>
+      </c>
+      <c r="AR201" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS201" t="n">
+        <v>0</v>
+      </c>
+      <c r="AT201" t="n">
+        <v>0</v>
+      </c>
+      <c r="AU201" t="b">
+        <v>0</v>
+      </c>
+      <c r="AV201" t="inlineStr">
+        <is>
+          <t>Standard</t>
+        </is>
+      </c>
+      <c r="AW201" t="inlineStr">
+        <is>
+          <t>1785d8f2-b59f-42d5-b3d6-ae008e17e6dc</t>
+        </is>
+      </c>
+      <c r="AX201" t="inlineStr">
         <is>
           <t>has_been_archived</t>
         </is>

</xml_diff>

<commit_message>
Checks for integer only
</commit_message>
<xml_diff>
--- a/master_fantasy_book_list.xlsx
+++ b/master_fantasy_book_list.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\p\fantasy_books_workspace\fantasy_books\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F2741E4-D140-43D8-A6FC-41BD82470A8D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{850A2051-E1C8-4807-9D56-45C67F99AEB5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -580,8 +580,8 @@
     <col min="41" max="48" width="9.140625" style="1" customWidth="1"/>
     <col min="49" max="49" width="37.140625" style="1" customWidth="1"/>
     <col min="50" max="50" width="18.140625" style="1" customWidth="1"/>
-    <col min="51" max="73" width="9.140625" style="1" customWidth="1"/>
-    <col min="74" max="16384" width="9.140625" style="1"/>
+    <col min="51" max="74" width="9.140625" style="1" customWidth="1"/>
+    <col min="75" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:50" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Check for zeros in the request box.
</commit_message>
<xml_diff>
--- a/master_fantasy_book_list.xlsx
+++ b/master_fantasy_book_list.xlsx
@@ -456,7 +456,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AY224"/>
+  <dimension ref="A1:AX224"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
@@ -19472,7 +19472,7 @@
         <v>1951</v>
       </c>
       <c r="X118" t="n">
-        <v>1898</v>
+        <v>1897</v>
       </c>
       <c r="Y118" t="n">
         <v>0</v>

</xml_diff>

<commit_message>
Endless loop for low budget fixed.
</commit_message>
<xml_diff>
--- a/master_fantasy_book_list.xlsx
+++ b/master_fantasy_book_list.xlsx
@@ -4349,7 +4349,7 @@
         <v>1922</v>
       </c>
       <c r="X24" t="n">
-        <v>1876</v>
+        <v>1875</v>
       </c>
       <c r="Y24" t="n">
         <v>0</v>
@@ -7215,7 +7215,7 @@
         <v>1527</v>
       </c>
       <c r="X42" t="n">
-        <v>1487</v>
+        <v>1486</v>
       </c>
       <c r="Y42" t="n">
         <v>0</v>
@@ -8182,7 +8182,7 @@
         <v>433</v>
       </c>
       <c r="X48" t="n">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="Y48" t="n">
         <v>0.02</v>
@@ -13174,7 +13174,7 @@
         <v>748</v>
       </c>
       <c r="X79" t="n">
-        <v>728</v>
+        <v>727</v>
       </c>
       <c r="Y79" t="n">
         <v>0.01</v>
@@ -20738,7 +20738,7 @@
         <v>558</v>
       </c>
       <c r="X126" t="n">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="Y126" t="n">
         <v>0.01</v>

</xml_diff>

<commit_message>
All works after Dropbox issue
</commit_message>
<xml_diff>
--- a/master_fantasy_book_list.xlsx
+++ b/master_fantasy_book_list.xlsx
@@ -4349,7 +4349,7 @@
         <v>1922</v>
       </c>
       <c r="X24" t="n">
-        <v>1873</v>
+        <v>1872</v>
       </c>
       <c r="Y24" t="n">
         <v>0</v>
@@ -7215,7 +7215,7 @@
         <v>1527</v>
       </c>
       <c r="X42" t="n">
-        <v>1485</v>
+        <v>1484</v>
       </c>
       <c r="Y42" t="n">
         <v>0</v>
@@ -8835,7 +8835,7 @@
         <v>441</v>
       </c>
       <c r="X52" t="n">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="Y52" t="n">
         <v>0.02</v>
@@ -12536,7 +12536,7 @@
         <v>1001</v>
       </c>
       <c r="X75" t="n">
-        <v>975</v>
+        <v>974</v>
       </c>
       <c r="Y75" t="n">
         <v>0</v>
@@ -13822,7 +13822,7 @@
         <v>1459</v>
       </c>
       <c r="X83" t="n">
-        <v>1420</v>
+        <v>1419</v>
       </c>
       <c r="Y83" t="n">
         <v>0</v>
@@ -16556,7 +16556,7 @@
         <v>496</v>
       </c>
       <c r="X100" t="n">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="Y100" t="n">
         <v>0.02</v>
@@ -18520,7 +18520,7 @@
         <v>635</v>
       </c>
       <c r="X112" t="n">
-        <v>618</v>
+        <v>617</v>
       </c>
       <c r="Y112" t="n">
         <v>0.01</v>
@@ -19472,7 +19472,7 @@
         <v>1951</v>
       </c>
       <c r="X118" t="n">
-        <v>1896</v>
+        <v>1895</v>
       </c>
       <c r="Y118" t="n">
         <v>0</v>
@@ -27118,7 +27118,7 @@
         <v>1274</v>
       </c>
       <c r="X166" t="n">
-        <v>1246</v>
+        <v>1244</v>
       </c>
       <c r="Y166" t="n">
         <v>0</v>
@@ -35517,7 +35517,7 @@
         <v>217</v>
       </c>
       <c r="X218" t="n">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="Y218" t="n">
         <v>0.05</v>

</xml_diff>